<commit_message>
Updated fixtures with newest data from xiaomi.eu 2 new devices, 5 new weekly folders
</commit_message>
<xml_diff>
--- a/XiaomiEuRomChecker/core/initial_devices_list.xlsx
+++ b/XiaomiEuRomChecker/core/initial_devices_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\PycharmProjects\XiaomiEuRomChecker\XiaomiEuRomChecker\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{546037ED-718E-43B4-BEE9-76BB11EA6FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FEB8C52-16DB-417E-AC90-812B716E9277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5CAD35A0-99CB-4F38-9642-5A6AB9CEA1C4}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="278">
   <si>
     <t>code_name</t>
   </si>
@@ -623,9 +624,6 @@
     <t>weekly</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
     <t>slug</t>
   </si>
   <si>
@@ -852,13 +850,34 @@
   </si>
   <si>
     <t>redmi-note-12-5g</t>
+  </si>
+  <si>
+    <t>peux</t>
+  </si>
+  <si>
+    <t>peux_p</t>
+  </si>
+  <si>
+    <t>Redmi Note 11 Pro+ 5G (India)</t>
+  </si>
+  <si>
+    <t>VEUXG</t>
+  </si>
+  <si>
+    <t>redmi-note-11-pro-5g-india</t>
+  </si>
+  <si>
+    <t>POCO X4 Pro 5G (India 64MP)</t>
+  </si>
+  <si>
+    <t>poco-x4-pro-5g-india-64mp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -876,8 +895,12 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -896,8 +919,14 @@
         <bgColor theme="5" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -951,11 +980,73 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -967,13 +1058,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="5"/>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="5" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="5" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="5" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="5" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="5" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="5" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="5" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="5" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="5" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="5" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="5" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -987,17 +1207,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5EA61572-5A57-4922-9E96-78091F40284C}" name="Table13" displayName="Table13" ref="A1:E1048576" totalsRowShown="0">
-  <autoFilter ref="A1:E1048576" xr:uid="{5EA61572-5A57-4922-9E96-78091F40284C}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{776FE8E6-49C2-4261-A75B-D9FF34CE5A6F}" name="code_name"/>
-    <tableColumn id="2" xr3:uid="{983A5B7A-C7BA-41EC-B07D-4585094C2851}" name="market_name"/>
-    <tableColumn id="3" xr3:uid="{0830D650-2611-4EC6-B7D6-8A965CA4A6FD}" name="rom_name"/>
-    <tableColumn id="6" xr3:uid="{2DEC9862-18F9-40EC-8BAE-392001E8D94D}" name="rom_version"/>
-    <tableColumn id="7" xr3:uid="{48AA6F4D-5A88-448D-8A4A-CD91B0A47601}" name="slug"/>
-    <tableColumn id="4" xr3:uid="{FCC7E686-B3E6-4398-A824-8C7FE0CE5C60}" name="Column1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20CE392A-2600-4684-9B70-930EF9E57E57}" name="Table1" displayName="Table1" ref="A1:E78" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:E78" xr:uid="{20CE392A-2600-4684-9B70-930EF9E57E57}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{D83EA653-F62B-4487-8413-9C6EEDD89C17}" name="code_name" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{FB28373B-6B93-476B-84EC-EAB8BE17962E}" name="market_name" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{9BBDB551-4826-46A3-8735-F2AA5BCE228C}" name="rom_name" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{0FE6270C-857B-4B4D-BBB0-19F2D7D7C17F}" name="rom_version" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{4D8789E0-BA26-4F50-855F-735A9388B9D1}" name="slug" dataDxfId="1"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1298,10 +1517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0006AD9-E68C-4EA4-BC75-8DF486AEC5F0}">
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,7 +1546,7 @@
         <v>146</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1344,7 +1563,7 @@
         <v>147</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1361,7 +1580,7 @@
         <v>147</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1378,7 +1597,7 @@
         <v>147</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1395,7 +1614,7 @@
         <v>147</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1412,7 +1631,7 @@
         <v>147</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1429,7 +1648,7 @@
         <v>147</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1446,7 +1665,7 @@
         <v>147</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1463,7 +1682,7 @@
         <v>147</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1480,7 +1699,7 @@
         <v>147</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1497,7 +1716,7 @@
         <v>147</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1514,7 +1733,7 @@
         <v>147</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1531,7 +1750,7 @@
         <v>192</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1548,7 +1767,7 @@
         <v>147</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1565,7 +1784,7 @@
         <v>147</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1582,7 +1801,7 @@
         <v>192</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1599,7 +1818,7 @@
         <v>192</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1616,7 +1835,7 @@
         <v>192</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1633,7 +1852,7 @@
         <v>147</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1650,7 +1869,7 @@
         <v>147</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1667,7 +1886,7 @@
         <v>147</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1684,7 +1903,7 @@
         <v>147</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1701,7 +1920,7 @@
         <v>147</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1718,7 +1937,7 @@
         <v>147</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1735,7 +1954,7 @@
         <v>192</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1752,7 +1971,7 @@
         <v>192</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1769,7 +1988,7 @@
         <v>192</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1786,7 +2005,7 @@
         <v>147</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1803,7 +2022,7 @@
         <v>147</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1820,7 +2039,7 @@
         <v>147</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1837,7 +2056,7 @@
         <v>147</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1854,7 +2073,7 @@
         <v>147</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1871,7 +2090,7 @@
         <v>147</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1888,7 +2107,7 @@
         <v>147</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1905,7 +2124,7 @@
         <v>147</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1922,7 +2141,7 @@
         <v>147</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1939,7 +2158,7 @@
         <v>147</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1956,7 +2175,7 @@
         <v>147</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1973,7 +2192,7 @@
         <v>147</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1990,7 +2209,7 @@
         <v>192</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2007,7 +2226,7 @@
         <v>192</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -2024,7 +2243,7 @@
         <v>147</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -2041,7 +2260,7 @@
         <v>192</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2058,7 +2277,7 @@
         <v>194</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -2075,7 +2294,7 @@
         <v>147</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -2092,7 +2311,7 @@
         <v>192</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -2109,7 +2328,7 @@
         <v>192</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -2126,483 +2345,517 @@
         <v>192</v>
       </c>
       <c r="E48" s="12" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="C49" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="D49" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B50" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="C50" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D50" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="22" t="s">
+        <v>271</v>
+      </c>
+      <c r="B51" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="C51" s="23" t="s">
+        <v>274</v>
+      </c>
+      <c r="D51" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="E51" s="13" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="22" t="s">
+        <v>272</v>
+      </c>
+      <c r="B52" s="23" t="s">
+        <v>276</v>
+      </c>
+      <c r="C52" s="23" t="s">
+        <v>274</v>
+      </c>
+      <c r="D52" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="E52" s="13" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B53" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="C53" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="D53" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="E53" s="12" t="s">
         <v>230</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="E49" s="12" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="E50" s="12" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="E51" s="12" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="E52" s="12" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="E53" s="12" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>147</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>192</v>
+        <v>147</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>232</v>
+        <v>261</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>147</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>147</v>
+        <v>192</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>251</v>
+        <v>231</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>192</v>
+        <v>147</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>233</v>
+        <v>262</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>147</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>147</v>
+        <v>192</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>271</v>
+        <v>232</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>94</v>
+        <v>161</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>147</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>252</v>
+        <v>263</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>147</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>179</v>
+        <v>94</v>
       </c>
       <c r="D63" s="6" t="s">
         <v>147</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>147</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>234</v>
+        <v>264</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>147</v>
       </c>
       <c r="E65" s="12" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="C66" s="9" t="s">
-        <v>181</v>
+        <v>165</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>180</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>192</v>
+        <v>147</v>
       </c>
       <c r="E66" s="12" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>147</v>
       </c>
       <c r="E67" s="12" t="s">
-        <v>236</v>
+        <v>266</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>147</v>
+        <v>192</v>
       </c>
       <c r="E68" s="12" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D69" s="6" t="s">
         <v>147</v>
       </c>
       <c r="E69" s="12" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>192</v>
+        <v>147</v>
       </c>
       <c r="E70" s="12" t="s">
-        <v>238</v>
+        <v>252</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>80</v>
+        <v>186</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>147</v>
       </c>
       <c r="E71" s="12" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D72" s="6" t="s">
         <v>192</v>
       </c>
       <c r="E72" s="12" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>183</v>
+        <v>80</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>147</v>
       </c>
       <c r="E73" s="12" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>147</v>
+        <v>192</v>
       </c>
       <c r="E74" s="12" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>192</v>
+        <v>147</v>
       </c>
       <c r="E75" s="12" t="s">
-        <v>241</v>
+        <v>254</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E76" s="12" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C77" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="E77" s="12" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B78" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="C76" s="9" t="s">
+      <c r="C78" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="D76" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="E76" s="12" t="s">
-        <v>242</v>
+      <c r="D78" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E78" s="12" t="s">
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>